<commit_message>
finalizacao de normalizacao dos dados e salvamento em planilha
</commit_message>
<xml_diff>
--- a/MLP/Dados.xlsx
+++ b/MLP/Dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07a43a5b2b7678a4/Desktop/Aulas BCC/CC56A - Int. Art/Projeto Final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07a43a5b2b7678a4/Desktop/Aulas BCC/CC56A - Int. Art/Projeto Final/MLP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{231BAA59-44D3-4C10-9E10-365A006AEE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{734E4894-6724-46B4-B3A1-A7097EA445D8}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{231BAA59-44D3-4C10-9E10-365A006AEE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12D18A48-9768-4E58-9114-A97403CF3120}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="-8510" windowWidth="10980" windowHeight="9330" xr2:uid="{ABEC26F5-C8BE-4E69-AF24-DB461A37DE22}"/>
+    <workbookView xWindow="590" yWindow="730" windowWidth="10980" windowHeight="9350" xr2:uid="{ABEC26F5-C8BE-4E69-AF24-DB461A37DE22}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="17">
   <si>
     <t>CABELO</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>AZUL</t>
-  </si>
-  <si>
-    <t>NÃO</t>
   </si>
   <si>
     <t>VERDE</t>
@@ -131,7 +128,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -147,6 +144,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BBD9FD-2CA6-45C2-970D-1E0003D5B94A}">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113:B121"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -483,7 +484,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -503,7 +504,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -523,7 +524,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -543,7 +544,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -563,7 +564,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -583,7 +584,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -603,7 +604,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -623,7 +624,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -643,7 +644,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -663,7 +664,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -683,7 +684,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -692,7 +693,7 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
@@ -703,7 +704,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -723,7 +724,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -743,7 +744,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -763,7 +764,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
@@ -783,7 +784,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -803,7 +804,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
@@ -812,7 +813,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -823,7 +824,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -843,7 +844,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
@@ -863,7 +864,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
@@ -883,7 +884,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -903,7 +904,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
@@ -923,7 +924,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
@@ -943,7 +944,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
@@ -963,7 +964,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
@@ -983,7 +984,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -992,7 +993,7 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27" t="s">
         <v>9</v>
@@ -1023,7 +1024,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
@@ -1043,7 +1044,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
@@ -1063,7 +1064,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
@@ -1083,7 +1084,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
@@ -1092,7 +1093,7 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
@@ -1123,7 +1124,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
         <v>4</v>
@@ -1132,7 +1133,7 @@
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E34" t="s">
         <v>9</v>
@@ -1163,7 +1164,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
@@ -1183,7 +1184,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
@@ -1203,7 +1204,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
         <v>4</v>
@@ -1215,7 +1216,7 @@
         <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -1223,7 +1224,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
@@ -1243,10 +1244,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>15</v>
-      </c>
-      <c r="B40" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
@@ -1263,7 +1264,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>
@@ -1283,7 +1284,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
         <v>4</v>
@@ -1303,7 +1304,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
@@ -1323,7 +1324,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
@@ -1343,7 +1344,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
         <v>4</v>
@@ -1363,7 +1364,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
@@ -1383,7 +1384,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
@@ -1403,7 +1404,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B48" t="s">
         <v>4</v>
@@ -1423,7 +1424,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B49" t="s">
         <v>4</v>
@@ -1443,7 +1444,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B50" t="s">
         <v>4</v>
@@ -1463,7 +1464,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B51" t="s">
         <v>4</v>
@@ -1483,7 +1484,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
         <v>4</v>
@@ -1503,7 +1504,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
         <v>4</v>
@@ -1543,7 +1544,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B55" t="s">
         <v>4</v>
@@ -1563,7 +1564,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B56" t="s">
         <v>4</v>
@@ -1575,7 +1576,7 @@
         <v>6</v>
       </c>
       <c r="E56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -1583,7 +1584,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B57" t="s">
         <v>4</v>
@@ -1603,7 +1604,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B58" t="s">
         <v>4</v>
@@ -1623,7 +1624,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B59" t="s">
         <v>4</v>
@@ -1632,7 +1633,7 @@
         <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E59" t="s">
         <v>9</v>
@@ -1643,7 +1644,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B60" t="s">
         <v>4</v>
@@ -1663,7 +1664,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B61" t="s">
         <v>4</v>
@@ -1683,7 +1684,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B62" t="s">
         <v>4</v>
@@ -1706,16 +1707,16 @@
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C63" t="s">
         <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -1726,16 +1727,16 @@
         <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C64" t="s">
         <v>8</v>
       </c>
       <c r="D64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -1746,16 +1747,16 @@
         <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C65" t="s">
         <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -1766,13 +1767,13 @@
         <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C66" t="s">
         <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E66" t="s">
         <v>9</v>
@@ -1786,16 +1787,16 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C67" t="s">
         <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -1806,7 +1807,7 @@
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C68" t="s">
         <v>10</v>
@@ -1815,7 +1816,7 @@
         <v>6</v>
       </c>
       <c r="E68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -1826,16 +1827,16 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C69" t="s">
         <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -1846,16 +1847,16 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C70" t="s">
         <v>10</v>
       </c>
       <c r="D70" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -1866,16 +1867,16 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C71" t="s">
         <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E71" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -1886,13 +1887,13 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C72" t="s">
         <v>10</v>
       </c>
       <c r="D72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E72" t="s">
         <v>9</v>
@@ -1906,16 +1907,16 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C73" t="s">
         <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E73" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -1926,16 +1927,16 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C74" t="s">
         <v>10</v>
       </c>
       <c r="D74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E74" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -1946,16 +1947,16 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C75" t="s">
         <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E75" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -1966,16 +1967,16 @@
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C76" t="s">
         <v>10</v>
       </c>
       <c r="D76" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E76" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -1986,13 +1987,13 @@
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C77" t="s">
         <v>10</v>
       </c>
       <c r="D77" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E77" t="s">
         <v>9</v>
@@ -2006,7 +2007,7 @@
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
@@ -2026,16 +2027,16 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C79" t="s">
         <v>10</v>
       </c>
       <c r="D79" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E79" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -2046,13 +2047,13 @@
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C80" t="s">
         <v>8</v>
       </c>
       <c r="D80" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E80" t="s">
         <v>9</v>
@@ -2086,13 +2087,13 @@
         <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C82" t="s">
         <v>10</v>
       </c>
       <c r="D82" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E82" t="s">
         <v>9</v>
@@ -2106,13 +2107,13 @@
         <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C83" t="s">
         <v>8</v>
       </c>
       <c r="D83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E83" t="s">
         <v>9</v>
@@ -2126,16 +2127,16 @@
         <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C84" t="s">
         <v>10</v>
       </c>
       <c r="D84" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E84" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F84">
         <v>0</v>
@@ -2146,13 +2147,13 @@
         <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
       </c>
       <c r="D85" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E85" t="s">
         <v>9</v>
@@ -2166,13 +2167,13 @@
         <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C86" t="s">
         <v>10</v>
       </c>
       <c r="D86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E86" t="s">
         <v>9</v>
@@ -2186,7 +2187,7 @@
         <v>11</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>8</v>
@@ -2203,7 +2204,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>4</v>
@@ -2223,7 +2224,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>4</v>
@@ -2243,7 +2244,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>4</v>
@@ -2263,10 +2264,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>8</v>
@@ -2283,7 +2284,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>4</v>
@@ -2303,7 +2304,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>4</v>
@@ -2323,7 +2324,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>4</v>
@@ -2343,7 +2344,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>4</v>
@@ -2363,7 +2364,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>4</v>
@@ -2383,7 +2384,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>4</v>
@@ -2403,7 +2404,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>4</v>
@@ -2423,7 +2424,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>4</v>
@@ -2443,7 +2444,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>4</v>
@@ -2463,7 +2464,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>4</v>
@@ -2483,7 +2484,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>4</v>
@@ -2503,7 +2504,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>4</v>
@@ -2523,7 +2524,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>4</v>
@@ -2543,7 +2544,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>4</v>
@@ -2563,7 +2564,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>4</v>
@@ -2583,7 +2584,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>4</v>
@@ -2603,7 +2604,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>4</v>
@@ -2623,7 +2624,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>4</v>
@@ -2635,7 +2636,7 @@
         <v>6</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F109" s="1">
         <v>1</v>
@@ -2643,7 +2644,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>4</v>
@@ -2663,7 +2664,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>4</v>
@@ -2695,7 +2696,7 @@
         <v>6</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F112" s="1">
         <v>0</v>
@@ -2705,14 +2706,14 @@
       <c r="A113" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>17</v>
+      <c r="B113" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>9</v>
@@ -2725,17 +2726,17 @@
       <c r="A114" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>17</v>
+      <c r="B114" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F114" s="1">
         <v>0</v>
@@ -2745,14 +2746,14 @@
       <c r="A115" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>17</v>
+      <c r="B115" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>9</v>
@@ -2765,17 +2766,17 @@
       <c r="A116" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>17</v>
+      <c r="B116" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F116" s="1">
         <v>0</v>
@@ -2785,17 +2786,17 @@
       <c r="A117" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>17</v>
+      <c r="B117" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F117" s="1">
         <v>0</v>
@@ -2805,14 +2806,14 @@
       <c r="A118" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B118" s="2" t="s">
-        <v>17</v>
+      <c r="B118" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>9</v>
@@ -2825,17 +2826,17 @@
       <c r="A119" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>17</v>
+      <c r="B119" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F119" s="1">
         <v>0</v>
@@ -2845,14 +2846,14 @@
       <c r="A120" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>17</v>
+      <c r="B120" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>9</v>
@@ -2865,14 +2866,14 @@
       <c r="A121" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B121" s="2" t="s">
-        <v>17</v>
+      <c r="B121" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>9</v>

</xml_diff>